<commit_message>
Ajustes para ler dados do Padilha
</commit_message>
<xml_diff>
--- a/data/instances/Analise Instancias.xlsx
+++ b/data/instances/Analise Instancias.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcio Barros\Documents\GitHub\Hector\data\instances\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="BOLS" sheetId="4" r:id="rId3"/>
     <sheet name="ACAD" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1580,7 +1585,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1615,7 +1620,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1828,7 +1833,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3417,7 +3422,7 @@
         <v>2</v>
       </c>
       <c r="D54">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="4"/>
@@ -3425,7 +3430,7 @@
       </c>
       <c r="G54" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="s">
         <v>68</v>
@@ -3448,7 +3453,7 @@
         <v>2</v>
       </c>
       <c r="D55">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="4"/>
@@ -3456,7 +3461,7 @@
       </c>
       <c r="G55" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" t="s">
         <v>73</v>
@@ -3541,7 +3546,7 @@
         <v>2</v>
       </c>
       <c r="D58">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="4"/>
@@ -3549,7 +3554,7 @@
       </c>
       <c r="G58" s="1">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I58" t="s">
         <v>94</v>
@@ -3603,7 +3608,7 @@
         <v>2</v>
       </c>
       <c r="D60">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="4"/>
@@ -3611,7 +3616,7 @@
       </c>
       <c r="G60" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="s">
         <v>118</v>
@@ -3665,7 +3670,7 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F62" s="1">
         <f t="shared" si="4"/>
@@ -3673,7 +3678,7 @@
       </c>
       <c r="G62" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" t="s">
         <v>108</v>
@@ -3696,7 +3701,7 @@
         <v>2</v>
       </c>
       <c r="D63">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" s="1">
         <f t="shared" si="4"/>
@@ -3704,7 +3709,7 @@
       </c>
       <c r="G63" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" t="s">
         <v>84</v>
@@ -3820,7 +3825,7 @@
         <v>2</v>
       </c>
       <c r="D67">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" s="1">
         <f t="shared" si="4"/>
@@ -3828,7 +3833,7 @@
       </c>
       <c r="G67" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" t="s">
         <v>74</v>
@@ -4192,7 +4197,7 @@
         <v>2</v>
       </c>
       <c r="D79">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" s="1">
         <f t="shared" si="4"/>
@@ -4200,7 +4205,7 @@
       </c>
       <c r="G79" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" t="s">
         <v>57</v>
@@ -4223,7 +4228,7 @@
         <v>2</v>
       </c>
       <c r="D80">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" s="1">
         <f t="shared" si="4"/>
@@ -4231,7 +4236,7 @@
       </c>
       <c r="G80" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80" t="s">
         <v>82</v>
@@ -4502,7 +4507,7 @@
         <v>1</v>
       </c>
       <c r="D89">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F89" s="1">
         <f t="shared" si="4"/>
@@ -4510,7 +4515,7 @@
       </c>
       <c r="G89" s="1">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>-5</v>
       </c>
       <c r="I89" t="s">
         <v>75</v>
@@ -4657,7 +4662,7 @@
         <v>2</v>
       </c>
       <c r="D94">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F94" s="1">
         <f t="shared" si="6"/>
@@ -4665,7 +4670,7 @@
       </c>
       <c r="G94" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I94" t="s">
         <v>55</v>
@@ -4688,7 +4693,7 @@
         <v>2</v>
       </c>
       <c r="D95">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F95" s="1">
         <f t="shared" si="6"/>
@@ -4696,7 +4701,7 @@
       </c>
       <c r="G95" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I95" t="s">
         <v>80</v>
@@ -4719,7 +4724,7 @@
         <v>2</v>
       </c>
       <c r="D96">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F96" s="1">
         <f t="shared" si="6"/>
@@ -4727,7 +4732,7 @@
       </c>
       <c r="G96" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" t="s">
         <v>21</v>
@@ -4750,7 +4755,7 @@
         <v>2</v>
       </c>
       <c r="D97">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F97" s="1">
         <f t="shared" si="6"/>
@@ -4758,7 +4763,7 @@
       </c>
       <c r="G97" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97" t="s">
         <v>85</v>
@@ -4781,7 +4786,7 @@
         <v>2</v>
       </c>
       <c r="D98">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F98" s="1">
         <f t="shared" si="6"/>
@@ -4789,7 +4794,7 @@
       </c>
       <c r="G98" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I98" t="s">
         <v>34</v>
@@ -4812,7 +4817,7 @@
         <v>2</v>
       </c>
       <c r="D99">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" s="1">
         <f t="shared" si="6"/>
@@ -4820,7 +4825,7 @@
       </c>
       <c r="G99" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I99" t="s">
         <v>113</v>
@@ -5560,7 +5565,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5599,7 +5604,7 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F11" si="0">C3-VLOOKUP(B3,$I$3:$K$11,2,FALSE)</f>
@@ -5607,7 +5612,7 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G11" si="1">D3-VLOOKUP(B3,$I$3:$K$11,3,FALSE)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="s">
         <v>130</v>
@@ -5878,7 +5883,7 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F13" s="1">
         <f>C13-VLOOKUP(B13,$I$13:$K$77,2,FALSE)</f>
@@ -5886,7 +5891,7 @@
       </c>
       <c r="G13" s="1">
         <f>D13-VLOOKUP(B13,$I$13:$K$77,3,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I13" t="s">
         <v>149</v>
@@ -5909,7 +5914,7 @@
         <v>3</v>
       </c>
       <c r="D14">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" ref="F14:F77" si="2">C14-VLOOKUP(B14,$I$13:$K$77,2,FALSE)</f>
@@ -5917,7 +5922,7 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" ref="G14:G77" si="3">D14-VLOOKUP(B14,$I$13:$K$77,3,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I14" t="s">
         <v>193</v>
@@ -6033,7 +6038,7 @@
         <v>2</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="2"/>
@@ -6041,7 +6046,7 @@
       </c>
       <c r="G18" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="s">
         <v>138</v>
@@ -6095,7 +6100,7 @@
         <v>2</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="2"/>
@@ -6103,7 +6108,7 @@
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="s">
         <v>142</v>
@@ -6343,7 +6348,7 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="2"/>
@@ -6351,7 +6356,7 @@
       </c>
       <c r="G28" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="s">
         <v>195</v>
@@ -6498,7 +6503,7 @@
         <v>1</v>
       </c>
       <c r="D33">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="2"/>
@@ -6506,7 +6511,7 @@
       </c>
       <c r="G33" s="1">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I33" t="s">
         <v>159</v>
@@ -6591,7 +6596,7 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="2"/>
@@ -6599,7 +6604,7 @@
       </c>
       <c r="G36" s="1">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="s">
         <v>136</v>
@@ -6622,7 +6627,7 @@
         <v>2</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="2"/>
@@ -6630,7 +6635,7 @@
       </c>
       <c r="G37" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" t="s">
         <v>163</v>
@@ -7707,7 +7712,7 @@
         <v>3</v>
       </c>
       <c r="D72">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F72" s="1">
         <f t="shared" si="2"/>
@@ -7715,7 +7720,7 @@
       </c>
       <c r="G72" s="1">
         <f t="shared" si="3"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="I72" t="s">
         <v>177</v>
@@ -7738,7 +7743,7 @@
         <v>2</v>
       </c>
       <c r="D73">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" s="1">
         <f t="shared" si="2"/>
@@ -7746,7 +7751,7 @@
       </c>
       <c r="G73" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I73" t="s">
         <v>189</v>
@@ -7769,7 +7774,7 @@
         <v>2</v>
       </c>
       <c r="D74">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" s="1">
         <f t="shared" si="2"/>
@@ -7777,7 +7782,7 @@
       </c>
       <c r="G74" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" t="s">
         <v>181</v>
@@ -7800,7 +7805,7 @@
         <v>2</v>
       </c>
       <c r="D75">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" s="1">
         <f t="shared" si="2"/>
@@ -7808,7 +7813,7 @@
       </c>
       <c r="G75" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" t="s">
         <v>194</v>
@@ -7831,7 +7836,7 @@
         <v>2</v>
       </c>
       <c r="D76">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" s="1">
         <f t="shared" si="2"/>
@@ -7839,7 +7844,7 @@
       </c>
       <c r="G76" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76" t="s">
         <v>196</v>
@@ -7862,7 +7867,7 @@
         <v>2</v>
       </c>
       <c r="D77">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" s="1">
         <f t="shared" si="2"/>
@@ -7870,7 +7875,7 @@
       </c>
       <c r="G77" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77" t="s">
         <v>197</v>
@@ -15373,7 +15378,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15415,11 +15420,11 @@
         <v>37</v>
       </c>
       <c r="F3" s="1">
-        <f>C3-VLOOKUP(B3,$I$3:$K$9,2,FALSE)</f>
+        <f t="shared" ref="F3:F9" si="0">C3-VLOOKUP(B3,$I$3:$K$9,2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <f>D3-VLOOKUP(B3,$I$3:$K$9,3,FALSE)</f>
+        <f t="shared" ref="G3:G9" si="1">D3-VLOOKUP(B3,$I$3:$K$9,3,FALSE)</f>
         <v>0</v>
       </c>
       <c r="I3" t="s">
@@ -15446,11 +15451,11 @@
         <v>7</v>
       </c>
       <c r="F4" s="1">
-        <f>C4-VLOOKUP(B4,$I$3:$K$9,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <f>D4-VLOOKUP(B4,$I$3:$K$9,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I4" t="s">
@@ -15477,11 +15482,11 @@
         <v>5</v>
       </c>
       <c r="F5" s="1">
-        <f>C5-VLOOKUP(B5,$I$3:$K$9,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <f>D5-VLOOKUP(B5,$I$3:$K$9,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I5" t="s">
@@ -15508,11 +15513,11 @@
         <v>4</v>
       </c>
       <c r="F6" s="1">
-        <f>C6-VLOOKUP(B6,$I$3:$K$9,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <f>D6-VLOOKUP(B6,$I$3:$K$9,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I6" t="s">
@@ -15536,15 +15541,15 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="1">
-        <f>C7-VLOOKUP(B7,$I$3:$K$9,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <f>D7-VLOOKUP(B7,$I$3:$K$9,3,FALSE)</f>
-        <v>-1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="I7" t="s">
         <v>439</v>
@@ -15570,11 +15575,11 @@
         <v>7</v>
       </c>
       <c r="F8" s="1">
-        <f>C8-VLOOKUP(B8,$I$3:$K$9,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <f>D8-VLOOKUP(B8,$I$3:$K$9,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I8" t="s">
@@ -15601,11 +15606,11 @@
         <v>4</v>
       </c>
       <c r="F9" s="1">
-        <f>C9-VLOOKUP(B9,$I$3:$K$9,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <f>D9-VLOOKUP(B9,$I$3:$K$9,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I9" t="s">
@@ -15632,11 +15637,11 @@
         <v>30</v>
       </c>
       <c r="F11" s="1">
-        <f>C11-VLOOKUP(B11,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" ref="F11:F49" si="2">C11-VLOOKUP(B11,$I$11:$K$49,2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="G11" s="1">
-        <f>D11-VLOOKUP(B11,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" ref="G11:G49" si="3">D11-VLOOKUP(B11,$I$11:$K$49,3,FALSE)</f>
         <v>0</v>
       </c>
       <c r="I11" t="s">
@@ -15663,11 +15668,11 @@
         <v>32</v>
       </c>
       <c r="F12" s="1">
-        <f>C12-VLOOKUP(B12,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <f>D12-VLOOKUP(B12,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I12" t="s">
@@ -15694,11 +15699,11 @@
         <v>32</v>
       </c>
       <c r="F13" s="1">
-        <f>C13-VLOOKUP(B13,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <f>D13-VLOOKUP(B13,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I13" t="s">
@@ -15725,11 +15730,11 @@
         <v>6</v>
       </c>
       <c r="F14" s="1">
-        <f>C14-VLOOKUP(B14,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <f>D14-VLOOKUP(B14,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I14" t="s">
@@ -15756,11 +15761,11 @@
         <v>5</v>
       </c>
       <c r="F15" s="1">
-        <f>C15-VLOOKUP(B15,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G15" s="1">
-        <f>D15-VLOOKUP(B15,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I15" t="s">
@@ -15787,11 +15792,11 @@
         <v>4</v>
       </c>
       <c r="F16" s="1">
-        <f>C16-VLOOKUP(B16,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <f>D16-VLOOKUP(B16,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I16" t="s">
@@ -15818,11 +15823,11 @@
         <v>6</v>
       </c>
       <c r="F17" s="1">
-        <f>C17-VLOOKUP(B17,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <f>D17-VLOOKUP(B17,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I17" t="s">
@@ -15849,11 +15854,11 @@
         <v>9</v>
       </c>
       <c r="F18" s="1">
-        <f>C18-VLOOKUP(B18,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" s="1">
-        <f>D18-VLOOKUP(B18,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I18" t="s">
@@ -15880,11 +15885,11 @@
         <v>6</v>
       </c>
       <c r="F19" s="1">
-        <f>C19-VLOOKUP(B19,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G19" s="1">
-        <f>D19-VLOOKUP(B19,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I19" t="s">
@@ -15911,11 +15916,11 @@
         <v>6</v>
       </c>
       <c r="F20" s="1">
-        <f>C20-VLOOKUP(B20,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20" s="1">
-        <f>D20-VLOOKUP(B20,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I20" t="s">
@@ -15942,11 +15947,11 @@
         <v>6</v>
       </c>
       <c r="F21" s="1">
-        <f>C21-VLOOKUP(B21,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <f>D21-VLOOKUP(B21,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I21" t="s">
@@ -15970,15 +15975,15 @@
         <v>2</v>
       </c>
       <c r="D22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" s="1">
-        <f>C22-VLOOKUP(B22,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <f>D22-VLOOKUP(B22,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I22" t="s">
         <v>462</v>
@@ -16001,15 +16006,15 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" s="1">
-        <f>C23-VLOOKUP(B23,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G23" s="1">
-        <f>D23-VLOOKUP(B23,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I23" t="s">
         <v>454</v>
@@ -16032,15 +16037,15 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" s="1">
-        <f>C24-VLOOKUP(B24,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <f>D24-VLOOKUP(B24,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I24" t="s">
         <v>474</v>
@@ -16066,11 +16071,11 @@
         <v>8</v>
       </c>
       <c r="F25" s="1">
-        <f>C25-VLOOKUP(B25,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G25" s="1">
-        <f>D25-VLOOKUP(B25,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I25" t="s">
@@ -16094,15 +16099,15 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" s="1">
-        <f>C26-VLOOKUP(B26,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <f>D26-VLOOKUP(B26,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I26" t="s">
         <v>466</v>
@@ -16125,15 +16130,15 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" s="1">
-        <f>C27-VLOOKUP(B27,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <f>D27-VLOOKUP(B27,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I27" t="s">
         <v>458</v>
@@ -16156,15 +16161,15 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" s="1">
-        <f>C28-VLOOKUP(B28,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G28" s="1">
-        <f>D28-VLOOKUP(B28,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I28" t="s">
         <v>478</v>
@@ -16190,11 +16195,11 @@
         <v>4</v>
       </c>
       <c r="F29" s="1">
-        <f>C29-VLOOKUP(B29,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <f>D29-VLOOKUP(B29,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I29" t="s">
@@ -16218,15 +16223,15 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" s="1">
-        <f>C30-VLOOKUP(B30,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G30" s="1">
-        <f>D30-VLOOKUP(B30,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I30" t="s">
         <v>483</v>
@@ -16249,15 +16254,15 @@
         <v>2</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" s="1">
-        <f>C31-VLOOKUP(B31,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G31" s="1">
-        <f>D31-VLOOKUP(B31,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I31" t="s">
         <v>452</v>
@@ -16280,15 +16285,15 @@
         <v>2</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" s="1">
-        <f>C32-VLOOKUP(B32,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G32" s="1">
-        <f>D32-VLOOKUP(B32,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I32" t="s">
         <v>460</v>
@@ -16314,11 +16319,11 @@
         <v>4</v>
       </c>
       <c r="F33" s="1">
-        <f>C33-VLOOKUP(B33,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G33" s="1">
-        <f>D33-VLOOKUP(B33,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I33" t="s">
@@ -16345,11 +16350,11 @@
         <v>5</v>
       </c>
       <c r="F34" s="1">
-        <f>C34-VLOOKUP(B34,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G34" s="1">
-        <f>D34-VLOOKUP(B34,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I34" t="s">
@@ -16376,11 +16381,11 @@
         <v>5</v>
       </c>
       <c r="F35" s="1">
-        <f>C35-VLOOKUP(B35,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G35" s="1">
-        <f>D35-VLOOKUP(B35,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I35" t="s">
@@ -16407,11 +16412,11 @@
         <v>5</v>
       </c>
       <c r="F36" s="1">
-        <f>C36-VLOOKUP(B36,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G36" s="1">
-        <f>D36-VLOOKUP(B36,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I36" t="s">
@@ -16438,11 +16443,11 @@
         <v>3</v>
       </c>
       <c r="F37" s="1">
-        <f>C37-VLOOKUP(B37,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G37" s="1">
-        <f>D37-VLOOKUP(B37,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I37" t="s">
@@ -16466,15 +16471,15 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F38" s="1">
-        <f>C38-VLOOKUP(B38,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G38" s="1">
-        <f>D38-VLOOKUP(B38,$I$11:$K$49,3,FALSE)</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I38" t="s">
         <v>468</v>
@@ -16497,15 +16502,15 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F39" s="1">
-        <f>C39-VLOOKUP(B39,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G39" s="1">
-        <f>D39-VLOOKUP(B39,$I$11:$K$49,3,FALSE)</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I39" t="s">
         <v>449</v>
@@ -16528,15 +16533,15 @@
         <v>1</v>
       </c>
       <c r="D40">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F40" s="1">
-        <f>C40-VLOOKUP(B40,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G40" s="1">
-        <f>D40-VLOOKUP(B40,$I$11:$K$49,3,FALSE)</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I40" t="s">
         <v>480</v>
@@ -16562,11 +16567,11 @@
         <v>2</v>
       </c>
       <c r="F41" s="1">
-        <f>C41-VLOOKUP(B41,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G41" s="1">
-        <f>D41-VLOOKUP(B41,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I41" t="s">
@@ -16590,15 +16595,15 @@
         <v>2</v>
       </c>
       <c r="D42">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" s="1">
-        <f>C42-VLOOKUP(B42,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G42" s="1">
-        <f>D42-VLOOKUP(B42,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I42" t="s">
         <v>463</v>
@@ -16621,15 +16626,15 @@
         <v>2</v>
       </c>
       <c r="D43">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" s="1">
-        <f>C43-VLOOKUP(B43,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G43" s="1">
-        <f>D43-VLOOKUP(B43,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I43" t="s">
         <v>455</v>
@@ -16652,15 +16657,15 @@
         <v>2</v>
       </c>
       <c r="D44">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F44" s="1">
-        <f>C44-VLOOKUP(B44,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G44" s="1">
-        <f>D44-VLOOKUP(B44,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I44" t="s">
         <v>475</v>
@@ -16686,11 +16691,11 @@
         <v>4</v>
       </c>
       <c r="F45" s="1">
-        <f>C45-VLOOKUP(B45,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G45" s="1">
-        <f>D45-VLOOKUP(B45,$I$11:$K$49,3,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I45" t="s">
@@ -16714,15 +16719,15 @@
         <v>2</v>
       </c>
       <c r="D46">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" s="1">
-        <f>C46-VLOOKUP(B46,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G46" s="1">
-        <f>D46-VLOOKUP(B46,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I46" t="s">
         <v>459</v>
@@ -16745,15 +16750,15 @@
         <v>2</v>
       </c>
       <c r="D47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" s="1">
-        <f>C47-VLOOKUP(B47,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G47" s="1">
-        <f>D47-VLOOKUP(B47,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I47" t="s">
         <v>451</v>
@@ -16776,15 +16781,15 @@
         <v>2</v>
       </c>
       <c r="D48">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" s="1">
-        <f>C48-VLOOKUP(B48,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G48" s="1">
-        <f>D48-VLOOKUP(B48,$I$11:$K$49,3,FALSE)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I48" t="s">
         <v>479</v>
@@ -16807,15 +16812,15 @@
         <v>4</v>
       </c>
       <c r="D49">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F49" s="1">
-        <f>C49-VLOOKUP(B49,$I$11:$K$49,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G49" s="1">
-        <f>D49-VLOOKUP(B49,$I$11:$K$49,3,FALSE)</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I49" t="s">
         <v>471</v>

</xml_diff>